<commit_message>
Update CountryData.xlsx with latest country information
</commit_message>
<xml_diff>
--- a/public/CountryData.xlsx
+++ b/public/CountryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jittakorn.s\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30AEC76-D212-42AF-AF74-489EEFEBB02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76864AAB-5BD4-4CC3-AA0F-9BFA623F2DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2066,7 +2066,7 @@
   <dimension ref="A1:H295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,6 +2075,7 @@
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3009,7 +3010,7 @@
         <v>79</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G35" t="s">
         <v>561</v>
@@ -3437,7 +3438,7 @@
         <v>112</v>
       </c>
       <c r="F51">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G51" t="str">
         <f>IFERROR(IF(VLOOKUP(E51,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3518,7 +3519,7 @@
         <v>118</v>
       </c>
       <c r="F54">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G54" t="str">
         <f>IFERROR(IF(VLOOKUP(E54,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3626,7 +3627,7 @@
         <v>126</v>
       </c>
       <c r="F58">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G58" t="str">
         <f>IFERROR(IF(VLOOKUP(E58,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3707,7 +3708,7 @@
         <v>132</v>
       </c>
       <c r="F61">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G61" t="str">
         <f>IFERROR(IF(VLOOKUP(E61,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3788,7 +3789,7 @@
         <v>138</v>
       </c>
       <c r="F64">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G64" t="str">
         <f>IFERROR(IF(VLOOKUP(E64,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3842,7 +3843,7 @@
         <v>142</v>
       </c>
       <c r="F66">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G66" t="str">
         <f>IFERROR(IF(VLOOKUP(E66,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3896,7 +3897,7 @@
         <v>146</v>
       </c>
       <c r="F68">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G68" t="str">
         <f>IFERROR(IF(VLOOKUP(E68,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -3950,7 +3951,7 @@
         <v>150</v>
       </c>
       <c r="F70">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G70" t="str">
         <f>IFERROR(IF(VLOOKUP(E70,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4004,7 +4005,7 @@
         <v>154</v>
       </c>
       <c r="F72">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G72" t="str">
         <f>IFERROR(IF(VLOOKUP(E72,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4058,7 +4059,7 @@
         <v>158</v>
       </c>
       <c r="F74">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G74" t="str">
         <f>IFERROR(IF(VLOOKUP(E74,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4112,7 +4113,7 @@
         <v>162</v>
       </c>
       <c r="F76">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G76" t="str">
         <f>IFERROR(IF(VLOOKUP(E76,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4139,7 +4140,7 @@
         <v>164</v>
       </c>
       <c r="F77">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G77" t="str">
         <f>IFERROR(IF(VLOOKUP(E77,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4166,7 +4167,7 @@
         <v>166</v>
       </c>
       <c r="F78">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G78" t="str">
         <f>IFERROR(IF(VLOOKUP(E78,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4274,7 +4275,7 @@
         <v>174</v>
       </c>
       <c r="F82">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G82" t="str">
         <f>IFERROR(IF(VLOOKUP(E82,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4301,7 +4302,7 @@
         <v>176</v>
       </c>
       <c r="F83">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G83" t="str">
         <f>IFERROR(IF(VLOOKUP(E83,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4328,7 +4329,7 @@
         <v>178</v>
       </c>
       <c r="F84">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G84" t="str">
         <f>IFERROR(IF(VLOOKUP(E84,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4382,7 +4383,7 @@
         <v>182</v>
       </c>
       <c r="F86">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G86" t="str">
         <f>IFERROR(IF(VLOOKUP(E86,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4409,7 +4410,7 @@
         <v>184</v>
       </c>
       <c r="F87">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G87" t="str">
         <f>IFERROR(IF(VLOOKUP(E87,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4436,7 +4437,7 @@
         <v>186</v>
       </c>
       <c r="F88">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G88" t="str">
         <f>IFERROR(IF(VLOOKUP(E88,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4490,7 +4491,7 @@
         <v>190</v>
       </c>
       <c r="F90">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G90" t="str">
         <f>IFERROR(IF(VLOOKUP(E90,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -4544,7 +4545,7 @@
         <v>194</v>
       </c>
       <c r="F92">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G92" t="str">
         <f>IFERROR(IF(VLOOKUP(E92,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5021,7 +5022,7 @@
         <v>231</v>
       </c>
       <c r="F110">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G110" t="str">
         <f>IFERROR(IF(VLOOKUP(E110,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5505,7 +5506,7 @@
         <v>269</v>
       </c>
       <c r="F128">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G128" t="str">
         <f>IFERROR(IF(VLOOKUP(E128,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5640,7 +5641,7 @@
         <v>280</v>
       </c>
       <c r="F133">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G133" t="str">
         <f>IFERROR(IF(VLOOKUP(E133,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5694,7 +5695,7 @@
         <v>284</v>
       </c>
       <c r="F135">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G135" t="s">
         <v>561</v>
@@ -5774,7 +5775,7 @@
         <v>290</v>
       </c>
       <c r="F138">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G138" t="str">
         <f>IFERROR(IF(VLOOKUP(E138,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5801,7 +5802,7 @@
         <v>292</v>
       </c>
       <c r="F139">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G139" t="str">
         <f>IFERROR(IF(VLOOKUP(E139,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5828,7 +5829,7 @@
         <v>294</v>
       </c>
       <c r="F140">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G140" t="str">
         <f>IFERROR(IF(VLOOKUP(E140,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -5855,7 +5856,7 @@
         <v>296</v>
       </c>
       <c r="F141">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G141" t="s">
         <v>561</v>
@@ -5935,7 +5936,7 @@
         <v>302</v>
       </c>
       <c r="F144">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G144" t="str">
         <f>IFERROR(IF(VLOOKUP(E144,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -6016,7 +6017,7 @@
         <v>308</v>
       </c>
       <c r="F147">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G147" t="str">
         <f>IFERROR(IF(VLOOKUP(E147,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -6097,7 +6098,7 @@
         <v>314</v>
       </c>
       <c r="F150">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G150" t="s">
         <v>561</v>
@@ -6150,7 +6151,7 @@
         <v>318</v>
       </c>
       <c r="F152">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G152" t="str">
         <f>IFERROR(IF(VLOOKUP(E152,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -6285,7 +6286,7 @@
         <v>328</v>
       </c>
       <c r="F157">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G157" t="s">
         <v>561</v>
@@ -6392,7 +6393,7 @@
         <v>336</v>
       </c>
       <c r="F161">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G161" t="s">
         <v>561</v>
@@ -6418,7 +6419,7 @@
         <v>338</v>
       </c>
       <c r="F162">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G162" t="s">
         <v>561</v>
@@ -6444,7 +6445,7 @@
         <v>340</v>
       </c>
       <c r="F163">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G163" t="str">
         <f>IFERROR(IF(VLOOKUP(E163,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -6471,7 +6472,7 @@
         <v>342</v>
       </c>
       <c r="F164">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G164" t="s">
         <v>561</v>
@@ -6578,7 +6579,7 @@
         <v>350</v>
       </c>
       <c r="F168">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G168" t="s">
         <v>561</v>
@@ -6658,7 +6659,7 @@
         <v>356</v>
       </c>
       <c r="F171">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G171" t="s">
         <v>561</v>
@@ -6684,7 +6685,7 @@
         <v>358</v>
       </c>
       <c r="F172">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G172" t="s">
         <v>561</v>
@@ -6710,7 +6711,7 @@
         <v>360</v>
       </c>
       <c r="F173">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G173" t="s">
         <v>561</v>
@@ -8352,7 +8353,7 @@
         <v>482</v>
       </c>
       <c r="F234">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G234" t="str">
         <f>IFERROR(IF(VLOOKUP(E234,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8379,7 +8380,7 @@
         <v>484</v>
       </c>
       <c r="F235">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G235" t="str">
         <f>IFERROR(IF(VLOOKUP(E235,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8514,7 +8515,7 @@
         <v>494</v>
       </c>
       <c r="F240">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G240" t="str">
         <f>IFERROR(IF(VLOOKUP(E240,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8541,7 +8542,7 @@
         <v>110</v>
       </c>
       <c r="F241">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G241" t="str">
         <f>IFERROR(IF(VLOOKUP(E241,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8568,7 +8569,7 @@
         <v>112</v>
       </c>
       <c r="F242">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G242" t="str">
         <f>IFERROR(IF(VLOOKUP(E242,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8595,7 +8596,7 @@
         <v>116</v>
       </c>
       <c r="F243">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G243" t="str">
         <f>IFERROR(IF(VLOOKUP(E243,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8622,7 +8623,7 @@
         <v>118</v>
       </c>
       <c r="F244">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G244" t="str">
         <f>IFERROR(IF(VLOOKUP(E244,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8649,7 +8650,7 @@
         <v>120</v>
       </c>
       <c r="F245">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G245" t="str">
         <f>IFERROR(IF(VLOOKUP(E245,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8676,7 +8677,7 @@
         <v>126</v>
       </c>
       <c r="F246">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G246" t="str">
         <f>IFERROR(IF(VLOOKUP(E246,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8703,7 +8704,7 @@
         <v>130</v>
       </c>
       <c r="F247">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G247" t="str">
         <f>IFERROR(IF(VLOOKUP(E247,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8730,7 +8731,7 @@
         <v>132</v>
       </c>
       <c r="F248">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G248" t="str">
         <f>IFERROR(IF(VLOOKUP(E248,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8757,7 +8758,7 @@
         <v>138</v>
       </c>
       <c r="F249">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G249" t="str">
         <f>IFERROR(IF(VLOOKUP(E249,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8784,7 +8785,7 @@
         <v>146</v>
       </c>
       <c r="F250">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G250" t="str">
         <f>IFERROR(IF(VLOOKUP(E250,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8811,7 +8812,7 @@
         <v>150</v>
       </c>
       <c r="F251">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G251" t="str">
         <f>IFERROR(IF(VLOOKUP(E251,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8838,7 +8839,7 @@
         <v>154</v>
       </c>
       <c r="F252">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G252" t="str">
         <f>IFERROR(IF(VLOOKUP(E252,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8865,7 +8866,7 @@
         <v>158</v>
       </c>
       <c r="F253">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G253" t="str">
         <f>IFERROR(IF(VLOOKUP(E253,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8892,7 +8893,7 @@
         <v>162</v>
       </c>
       <c r="F254">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G254" t="str">
         <f>IFERROR(IF(VLOOKUP(E254,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8919,7 +8920,7 @@
         <v>164</v>
       </c>
       <c r="F255">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G255" t="str">
         <f>IFERROR(IF(VLOOKUP(E255,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8946,7 +8947,7 @@
         <v>166</v>
       </c>
       <c r="F256">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G256" t="str">
         <f>IFERROR(IF(VLOOKUP(E256,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -8973,7 +8974,7 @@
         <v>174</v>
       </c>
       <c r="F257">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G257" t="str">
         <f>IFERROR(IF(VLOOKUP(E257,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9000,7 +9001,7 @@
         <v>176</v>
       </c>
       <c r="F258">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G258" t="str">
         <f>IFERROR(IF(VLOOKUP(E258,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9027,7 +9028,7 @@
         <v>178</v>
       </c>
       <c r="F259">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G259" t="str">
         <f>IFERROR(IF(VLOOKUP(E259,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9054,7 +9055,7 @@
         <v>182</v>
       </c>
       <c r="F260">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G260" t="str">
         <f>IFERROR(IF(VLOOKUP(E260,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9081,7 +9082,7 @@
         <v>184</v>
       </c>
       <c r="F261">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G261" t="str">
         <f>IFERROR(IF(VLOOKUP(E261,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9108,7 +9109,7 @@
         <v>190</v>
       </c>
       <c r="F262">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G262" t="str">
         <f>IFERROR(IF(VLOOKUP(E262,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9135,7 +9136,7 @@
         <v>482</v>
       </c>
       <c r="F263">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G263" t="str">
         <f>IFERROR(IF(VLOOKUP(E263,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9162,7 +9163,7 @@
         <v>497</v>
       </c>
       <c r="F264">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G264" t="str">
         <f>IFERROR(IF(VLOOKUP(E264,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9189,7 +9190,7 @@
         <v>500</v>
       </c>
       <c r="F265">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G265" t="str">
         <f>IFERROR(IF(VLOOKUP(E265,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9216,7 +9217,7 @@
         <v>503</v>
       </c>
       <c r="F266">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G266" t="str">
         <f>IFERROR(IF(VLOOKUP(E266,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9243,7 +9244,7 @@
         <v>506</v>
       </c>
       <c r="F267">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G267" t="str">
         <f>IFERROR(IF(VLOOKUP(E267,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9270,7 +9271,7 @@
         <v>122</v>
       </c>
       <c r="F268">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G268" t="str">
         <f>IFERROR(IF(VLOOKUP(E268,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9297,7 +9298,7 @@
         <v>124</v>
       </c>
       <c r="F269">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G269" t="str">
         <f>IFERROR(IF(VLOOKUP(E269,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9324,7 +9325,7 @@
         <v>142</v>
       </c>
       <c r="F270">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G270" t="str">
         <f>IFERROR(IF(VLOOKUP(E270,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9351,7 +9352,7 @@
         <v>186</v>
       </c>
       <c r="F271">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G271" t="str">
         <f>IFERROR(IF(VLOOKUP(E271,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9378,7 +9379,7 @@
         <v>194</v>
       </c>
       <c r="F272">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G272" t="str">
         <f>IFERROR(IF(VLOOKUP(E272,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9405,7 +9406,7 @@
         <v>509</v>
       </c>
       <c r="F273">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="G273" t="str">
         <f>IFERROR(IF(VLOOKUP(E273,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9539,7 +9540,7 @@
         <v>520</v>
       </c>
       <c r="F278">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G278" t="str">
         <f>IFERROR(IF(VLOOKUP(E278,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9620,7 +9621,7 @@
         <v>527</v>
       </c>
       <c r="F281">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="G281" t="str">
         <f>IFERROR(IF(VLOOKUP(E281,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9647,7 +9648,7 @@
         <v>530</v>
       </c>
       <c r="F282">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G282" t="str">
         <f>IFERROR(IF(VLOOKUP(E282,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9944,7 +9945,7 @@
         <v>553</v>
       </c>
       <c r="F293">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G293" t="str">
         <f>IFERROR(IF(VLOOKUP(E293,#REF!,1,1), "No", "Yes"), "No")</f>
@@ -9971,7 +9972,7 @@
         <v>556</v>
       </c>
       <c r="F294">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G294" t="str">
         <f>IFERROR(IF(VLOOKUP(E294,#REF!,1,1), "No", "Yes"), "No")</f>

</xml_diff>